<commit_message>
feat: Automate token usage tracking in Excel
</commit_message>
<xml_diff>
--- a/llm_token_usage.xlsx
+++ b/llm_token_usage.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Token Usage" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,11 +421,69 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>GPT4o</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Gemini</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>LLaMA</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Conveyor_System_Controller</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>979</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9589</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Traffic_Light_Controller</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>804</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6819</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>